<commit_message>
Spot, GPU, Cones, Water & Lavatory
</commit_message>
<xml_diff>
--- a/data_manual.xlsx
+++ b/data_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E02E2-C373-4C0E-AFD4-1FC539A640A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5F7D90-B7AE-4B46-AA7C-0DD4B747FFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,19 +689,10 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="I5" s="3">
-        <v>550</v>
-      </c>
-      <c r="J5" s="3">
-        <v>450</v>
-      </c>
-      <c r="K5" s="3">
-        <f>960+(960-I5)</f>
-        <v>1370</v>
-      </c>
-      <c r="L5" s="3">
-        <v>450</v>
-      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" s="1">
         <v>0</v>
       </c>
@@ -822,7 +813,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="5">
@@ -840,12 +831,8 @@
         <f t="shared" si="2"/>
         <v>Chocks_Rear</v>
       </c>
-      <c r="I11" s="3">
-        <v>950</v>
-      </c>
-      <c r="J11" s="3">
-        <v>300</v>
-      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="1">
@@ -1027,7 +1014,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="5">
@@ -1038,12 +1025,8 @@
         <v>Deboard</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="I20" s="3">
-        <v>1380</v>
-      </c>
-      <c r="J20" s="3">
-        <v>180</v>
-      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="M20" s="1">
         <v>0</v>

</xml_diff>